<commit_message>
atualizando as informações do projeto de banco de dados
</commit_message>
<xml_diff>
--- a/documents/modelo_dados.xlsx
+++ b/documents/modelo_dados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Tabela: TaskTypes</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>ended_at</t>
+  </si>
+  <si>
+    <t>total_duration</t>
   </si>
 </sst>
 </file>
@@ -168,9 +171,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -184,6 +184,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,60 +493,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" style="1"/>
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -554,7 +559,7 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -563,12 +568,16 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="5">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
         <v>2.7083333333333334E-2</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -582,7 +591,7 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -591,12 +600,16 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="5">
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4">
         <v>5.9027777777777783E-2</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -610,7 +623,7 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -619,12 +632,16 @@
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="5">
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
         <v>0.1076388888888889</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -635,49 +652,77 @@
       <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="I7" s="5">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
         <v>0.20694444444444446</v>
+      </c>
+      <c r="J7" s="3">
+        <v>44923.333333333336</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="I8" s="5">
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="J8" s="3">
+        <v>44924.333333333336</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -691,16 +736,19 @@
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="4">
-        <v>44922.333333333336</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="3">
+        <v>44922.333333333336</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="4">
-        <v>44922.333333333336</v>
-      </c>
-      <c r="G13" s="1" t="s">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="G13" s="3">
+        <v>44922.333333333336</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -714,16 +762,19 @@
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="4">
-        <v>44922.333333333336</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="3">
+        <v>44922.333333333336</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="4">
-        <v>44922.333333333336</v>
-      </c>
-      <c r="G14" s="1" t="s">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="G14" s="3">
+        <v>44922.333333333336</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -737,42 +788,45 @@
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="4">
-        <v>44922.333333333336</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="3">
+        <v>44922.333333333336</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="4">
-        <v>44922.333333333336</v>
-      </c>
-      <c r="G15" s="1" t="s">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="G15" s="3">
+        <v>44922.333333333336</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -783,10 +837,10 @@
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>44922.333333333336</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -800,10 +854,10 @@
       <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>44923.333333333336</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -814,15 +868,15 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:K2"/>
-    <mergeCell ref="A11:G11"/>
     <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A11:H11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C20" r:id="rId1"/>

</xml_diff>